<commit_message>
compatible with topic management
</commit_message>
<xml_diff>
--- a/data/intent_emotion_mapping_COPD.xlsx
+++ b/data/intent_emotion_mapping_COPD.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="53">
   <si>
     <t xml:space="preserve">nb</t>
   </si>
@@ -173,6 +173,12 @@
   </si>
   <si>
     <t xml:space="preserve">confused_patient_handling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toy-next-question-id</t>
   </si>
 </sst>
 </file>
@@ -280,10 +286,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:A15"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4921875" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -825,6 +831,41 @@
         <v>1</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="K16" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>